<commit_message>
updating to print correct distributed values
</commit_message>
<xml_diff>
--- a/distributed/distributed_shots_close.xlsx
+++ b/distributed/distributed_shots_close.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,816 +455,1630 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>5627</v>
+        <v>5618</v>
       </c>
       <c r="D2" t="n">
-        <v>655</v>
+        <v>481</v>
       </c>
       <c r="E2" t="n">
-        <v>1212</v>
+        <v>1624</v>
       </c>
       <c r="F2" t="n">
-        <v>698</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2710</v>
+        <v>4552</v>
       </c>
       <c r="D3" t="n">
-        <v>1877</v>
+        <v>1397</v>
       </c>
       <c r="E3" t="n">
-        <v>2083</v>
+        <v>920</v>
       </c>
       <c r="F3" t="n">
-        <v>1522</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5636</v>
+        <v>5609</v>
       </c>
       <c r="D4" t="n">
-        <v>676</v>
+        <v>453</v>
       </c>
       <c r="E4" t="n">
-        <v>1214</v>
+        <v>1662</v>
       </c>
       <c r="F4" t="n">
-        <v>666</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2675</v>
+        <v>4563</v>
       </c>
       <c r="D5" t="n">
-        <v>1876</v>
+        <v>1358</v>
       </c>
       <c r="E5" t="n">
-        <v>2056</v>
+        <v>961</v>
       </c>
       <c r="F5" t="n">
-        <v>1585</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5589</v>
+        <v>5554</v>
       </c>
       <c r="D6" t="n">
-        <v>662</v>
+        <v>491</v>
       </c>
       <c r="E6" t="n">
-        <v>1236</v>
+        <v>1650</v>
       </c>
       <c r="F6" t="n">
-        <v>705</v>
+        <v>497</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2716</v>
+        <v>4621</v>
       </c>
       <c r="D7" t="n">
-        <v>1873</v>
+        <v>1400</v>
       </c>
       <c r="E7" t="n">
-        <v>2144</v>
+        <v>845</v>
       </c>
       <c r="F7" t="n">
-        <v>1459</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5556</v>
+        <v>5604</v>
       </c>
       <c r="D8" t="n">
-        <v>670</v>
+        <v>477</v>
       </c>
       <c r="E8" t="n">
-        <v>1265</v>
+        <v>1649</v>
       </c>
       <c r="F8" t="n">
-        <v>701</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2687</v>
+        <v>4605</v>
       </c>
       <c r="D9" t="n">
-        <v>1891</v>
+        <v>1412</v>
       </c>
       <c r="E9" t="n">
-        <v>1990</v>
+        <v>853</v>
       </c>
       <c r="F9" t="n">
-        <v>1624</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>5526</v>
+        <v>5595</v>
       </c>
       <c r="D10" t="n">
-        <v>673</v>
+        <v>484</v>
       </c>
       <c r="E10" t="n">
-        <v>1296</v>
+        <v>1621</v>
       </c>
       <c r="F10" t="n">
-        <v>697</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2705</v>
+        <v>4522</v>
       </c>
       <c r="D11" t="n">
-        <v>1906</v>
+        <v>1434</v>
       </c>
       <c r="E11" t="n">
-        <v>2095</v>
+        <v>910</v>
       </c>
       <c r="F11" t="n">
-        <v>1486</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5623</v>
+        <v>5554</v>
       </c>
       <c r="D12" t="n">
-        <v>642</v>
+        <v>506</v>
       </c>
       <c r="E12" t="n">
-        <v>1244</v>
+        <v>1653</v>
       </c>
       <c r="F12" t="n">
-        <v>683</v>
+        <v>479</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2757</v>
+        <v>4632</v>
       </c>
       <c r="D13" t="n">
-        <v>1890</v>
+        <v>1373</v>
       </c>
       <c r="E13" t="n">
-        <v>2019</v>
+        <v>878</v>
       </c>
       <c r="F13" t="n">
-        <v>1526</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5616</v>
+        <v>5630</v>
       </c>
       <c r="D14" t="n">
-        <v>675</v>
+        <v>466</v>
       </c>
       <c r="E14" t="n">
-        <v>1242</v>
+        <v>1621</v>
       </c>
       <c r="F14" t="n">
-        <v>659</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2719</v>
+        <v>4589</v>
       </c>
       <c r="D15" t="n">
-        <v>1914</v>
+        <v>1400</v>
       </c>
       <c r="E15" t="n">
-        <v>2058</v>
+        <v>925</v>
       </c>
       <c r="F15" t="n">
-        <v>1501</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5611</v>
+        <v>5615</v>
       </c>
       <c r="D16" t="n">
-        <v>659</v>
+        <v>450</v>
       </c>
       <c r="E16" t="n">
-        <v>1272</v>
+        <v>1641</v>
       </c>
       <c r="F16" t="n">
-        <v>650</v>
+        <v>486</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2698</v>
+        <v>4459</v>
       </c>
       <c r="D17" t="n">
-        <v>1915</v>
+        <v>1432</v>
       </c>
       <c r="E17" t="n">
-        <v>2088</v>
+        <v>937</v>
       </c>
       <c r="F17" t="n">
-        <v>1491</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5612</v>
+        <v>5601</v>
       </c>
       <c r="D18" t="n">
-        <v>661</v>
+        <v>485</v>
       </c>
       <c r="E18" t="n">
-        <v>1229</v>
+        <v>1613</v>
       </c>
       <c r="F18" t="n">
-        <v>690</v>
+        <v>493</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2677</v>
+        <v>4664</v>
       </c>
       <c r="D19" t="n">
-        <v>1914</v>
+        <v>1342</v>
       </c>
       <c r="E19" t="n">
-        <v>2147</v>
+        <v>881</v>
       </c>
       <c r="F19" t="n">
-        <v>1454</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5615</v>
+        <v>5554</v>
       </c>
       <c r="D20" t="n">
-        <v>647</v>
+        <v>500</v>
       </c>
       <c r="E20" t="n">
-        <v>1247</v>
+        <v>1664</v>
       </c>
       <c r="F20" t="n">
-        <v>683</v>
+        <v>474</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2724</v>
+        <v>4619</v>
       </c>
       <c r="D21" t="n">
-        <v>1888</v>
+        <v>1349</v>
       </c>
       <c r="E21" t="n">
-        <v>2073</v>
+        <v>932</v>
       </c>
       <c r="F21" t="n">
-        <v>1507</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5615</v>
+        <v>5530</v>
       </c>
       <c r="D22" t="n">
-        <v>630</v>
+        <v>489</v>
       </c>
       <c r="E22" t="n">
-        <v>1233</v>
+        <v>1706</v>
       </c>
       <c r="F22" t="n">
-        <v>714</v>
+        <v>467</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2734</v>
+        <v>4604</v>
       </c>
       <c r="D23" t="n">
-        <v>1918</v>
+        <v>1367</v>
       </c>
       <c r="E23" t="n">
-        <v>2053</v>
+        <v>924</v>
       </c>
       <c r="F23" t="n">
-        <v>1487</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>5573</v>
+        <v>5583</v>
       </c>
       <c r="D24" t="n">
-        <v>668</v>
+        <v>466</v>
       </c>
       <c r="E24" t="n">
-        <v>1265</v>
+        <v>1660</v>
       </c>
       <c r="F24" t="n">
-        <v>686</v>
+        <v>483</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2733</v>
+        <v>4668</v>
       </c>
       <c r="D25" t="n">
-        <v>1849</v>
+        <v>1359</v>
       </c>
       <c r="E25" t="n">
-        <v>2075</v>
+        <v>833</v>
       </c>
       <c r="F25" t="n">
-        <v>1535</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5524</v>
+        <v>5597</v>
       </c>
       <c r="D26" t="n">
-        <v>681</v>
+        <v>486</v>
       </c>
       <c r="E26" t="n">
-        <v>1277</v>
+        <v>1627</v>
       </c>
       <c r="F26" t="n">
-        <v>710</v>
+        <v>482</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2698</v>
+        <v>4604</v>
       </c>
       <c r="D27" t="n">
-        <v>1916</v>
+        <v>1367</v>
       </c>
       <c r="E27" t="n">
-        <v>2103</v>
+        <v>869</v>
       </c>
       <c r="F27" t="n">
-        <v>1475</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>5572</v>
+        <v>5641</v>
       </c>
       <c r="D28" t="n">
-        <v>685</v>
+        <v>500</v>
       </c>
       <c r="E28" t="n">
-        <v>1245</v>
+        <v>1606</v>
       </c>
       <c r="F28" t="n">
-        <v>690</v>
+        <v>445</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2753</v>
+        <v>4557</v>
       </c>
       <c r="D29" t="n">
-        <v>1893</v>
+        <v>1363</v>
       </c>
       <c r="E29" t="n">
-        <v>2010</v>
+        <v>929</v>
       </c>
       <c r="F29" t="n">
-        <v>1536</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>5524</v>
+        <v>5518</v>
       </c>
       <c r="D30" t="n">
-        <v>732</v>
+        <v>502</v>
       </c>
       <c r="E30" t="n">
-        <v>1229</v>
+        <v>1699</v>
       </c>
       <c r="F30" t="n">
-        <v>707</v>
+        <v>473</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2697</v>
+        <v>4521</v>
       </c>
       <c r="D31" t="n">
-        <v>1946</v>
+        <v>1464</v>
       </c>
       <c r="E31" t="n">
-        <v>2040</v>
+        <v>890</v>
       </c>
       <c r="F31" t="n">
-        <v>1509</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5575</v>
+        <v>5588</v>
       </c>
       <c r="D32" t="n">
-        <v>649</v>
+        <v>514</v>
       </c>
       <c r="E32" t="n">
-        <v>1289</v>
+        <v>1613</v>
       </c>
       <c r="F32" t="n">
-        <v>679</v>
+        <v>477</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2695</v>
+        <v>4577</v>
       </c>
       <c r="D33" t="n">
-        <v>1918</v>
+        <v>1408</v>
       </c>
       <c r="E33" t="n">
-        <v>2072</v>
+        <v>886</v>
       </c>
       <c r="F33" t="n">
-        <v>1507</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>5591</v>
+        <v>5575</v>
       </c>
       <c r="D34" t="n">
-        <v>699</v>
+        <v>497</v>
       </c>
       <c r="E34" t="n">
-        <v>1245</v>
+        <v>1625</v>
       </c>
       <c r="F34" t="n">
-        <v>657</v>
+        <v>495</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2693</v>
+        <v>4566</v>
       </c>
       <c r="D35" t="n">
-        <v>1864</v>
+        <v>1388</v>
       </c>
       <c r="E35" t="n">
-        <v>2129</v>
+        <v>923</v>
       </c>
       <c r="F35" t="n">
-        <v>1506</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5525</v>
+        <v>5516</v>
       </c>
       <c r="D36" t="n">
-        <v>686</v>
+        <v>473</v>
       </c>
       <c r="E36" t="n">
-        <v>1277</v>
+        <v>1730</v>
       </c>
       <c r="F36" t="n">
-        <v>704</v>
+        <v>473</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2723</v>
+        <v>4536</v>
       </c>
       <c r="D37" t="n">
-        <v>1931</v>
+        <v>1375</v>
       </c>
       <c r="E37" t="n">
-        <v>2093</v>
+        <v>948</v>
       </c>
       <c r="F37" t="n">
-        <v>1445</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1619411711.601447</v>
+        <v>1619752193.191894</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ibmq_rome</t>
+          <t>ibmq_athens</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>5609</v>
+        <v>5631</v>
       </c>
       <c r="D38" t="n">
-        <v>640</v>
+        <v>502</v>
       </c>
       <c r="E38" t="n">
+        <v>1621</v>
+      </c>
+      <c r="F38" t="n">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>4634</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1369</v>
+      </c>
+      <c r="E39" t="n">
+        <v>920</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>5586</v>
+      </c>
+      <c r="D40" t="n">
+        <v>512</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1660</v>
+      </c>
+      <c r="F40" t="n">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>4632</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1312</v>
+      </c>
+      <c r="E41" t="n">
+        <v>919</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>5541</v>
+      </c>
+      <c r="D42" t="n">
+        <v>509</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1643</v>
+      </c>
+      <c r="F42" t="n">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>4637</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1401</v>
+      </c>
+      <c r="E43" t="n">
+        <v>889</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>5558</v>
+      </c>
+      <c r="D44" t="n">
+        <v>482</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1661</v>
+      </c>
+      <c r="F44" t="n">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>4579</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1402</v>
+      </c>
+      <c r="E45" t="n">
+        <v>915</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>5591</v>
+      </c>
+      <c r="D46" t="n">
+        <v>476</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1633</v>
+      </c>
+      <c r="F46" t="n">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>4486</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1413</v>
+      </c>
+      <c r="E47" t="n">
+        <v>929</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>5567</v>
+      </c>
+      <c r="D48" t="n">
+        <v>456</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1699</v>
+      </c>
+      <c r="F48" t="n">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>4639</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1395</v>
+      </c>
+      <c r="E49" t="n">
+        <v>870</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>5522</v>
+      </c>
+      <c r="D50" t="n">
+        <v>488</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1693</v>
+      </c>
+      <c r="F50" t="n">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>4552</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1432</v>
+      </c>
+      <c r="E51" t="n">
+        <v>916</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>5678</v>
+      </c>
+      <c r="D52" t="n">
+        <v>478</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1588</v>
+      </c>
+      <c r="F52" t="n">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>4552</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1431</v>
+      </c>
+      <c r="E53" t="n">
+        <v>932</v>
+      </c>
+      <c r="F53" t="n">
         <v>1277</v>
       </c>
-      <c r="F38" t="n">
-        <v>666</v>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>5544</v>
+      </c>
+      <c r="D54" t="n">
+        <v>476</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1637</v>
+      </c>
+      <c r="F54" t="n">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>4585</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1369</v>
+      </c>
+      <c r="E55" t="n">
+        <v>906</v>
+      </c>
+      <c r="F55" t="n">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>5518</v>
+      </c>
+      <c r="D56" t="n">
+        <v>521</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1667</v>
+      </c>
+      <c r="F56" t="n">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>4620</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1398</v>
+      </c>
+      <c r="E57" t="n">
+        <v>897</v>
+      </c>
+      <c r="F57" t="n">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>5607</v>
+      </c>
+      <c r="D58" t="n">
+        <v>506</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1618</v>
+      </c>
+      <c r="F58" t="n">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>4632</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1348</v>
+      </c>
+      <c r="E59" t="n">
+        <v>907</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>5585</v>
+      </c>
+      <c r="D60" t="n">
+        <v>483</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1636</v>
+      </c>
+      <c r="F60" t="n">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>4623</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1381</v>
+      </c>
+      <c r="E61" t="n">
+        <v>885</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>5577</v>
+      </c>
+      <c r="D62" t="n">
+        <v>486</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1646</v>
+      </c>
+      <c r="F62" t="n">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>4593</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1396</v>
+      </c>
+      <c r="E63" t="n">
+        <v>867</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>5640</v>
+      </c>
+      <c r="D64" t="n">
+        <v>466</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1644</v>
+      </c>
+      <c r="F64" t="n">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>4583</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1370</v>
+      </c>
+      <c r="E65" t="n">
+        <v>865</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>5634</v>
+      </c>
+      <c r="D66" t="n">
+        <v>497</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1593</v>
+      </c>
+      <c r="F66" t="n">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>4572</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1379</v>
+      </c>
+      <c r="E67" t="n">
+        <v>937</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>5623</v>
+      </c>
+      <c r="D68" t="n">
+        <v>468</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1603</v>
+      </c>
+      <c r="F68" t="n">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>4522</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1427</v>
+      </c>
+      <c r="E69" t="n">
+        <v>948</v>
+      </c>
+      <c r="F69" t="n">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>5617</v>
+      </c>
+      <c r="D70" t="n">
+        <v>481</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1599</v>
+      </c>
+      <c r="F70" t="n">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>4607</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1347</v>
+      </c>
+      <c r="E71" t="n">
+        <v>915</v>
+      </c>
+      <c r="F71" t="n">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>5576</v>
+      </c>
+      <c r="D72" t="n">
+        <v>464</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1646</v>
+      </c>
+      <c r="F72" t="n">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>4499</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1362</v>
+      </c>
+      <c r="E73" t="n">
+        <v>953</v>
+      </c>
+      <c r="F73" t="n">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>5625</v>
+      </c>
+      <c r="D74" t="n">
+        <v>482</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1630</v>
+      </c>
+      <c r="F74" t="n">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>1619752193.191894</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>ibmq_athens</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>4630</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1368</v>
+      </c>
+      <c r="E75" t="n">
+        <v>864</v>
+      </c>
+      <c r="F75" t="n">
+        <v>1330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trying with 20 shots
</commit_message>
<xml_diff>
--- a/distributed/distributed_shots_close.xlsx
+++ b/distributed/distributed_shots_close.xlsx
@@ -455,7 +455,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -463,21 +463,21 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>5618</v>
+        <v>7193</v>
       </c>
       <c r="D2" t="n">
-        <v>481</v>
+        <v>274</v>
       </c>
       <c r="E2" t="n">
-        <v>1624</v>
+        <v>505</v>
       </c>
       <c r="F2" t="n">
-        <v>469</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -485,21 +485,21 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4552</v>
+        <v>7130</v>
       </c>
       <c r="D3" t="n">
-        <v>1397</v>
+        <v>409</v>
       </c>
       <c r="E3" t="n">
-        <v>920</v>
+        <v>315</v>
       </c>
       <c r="F3" t="n">
-        <v>1323</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -507,21 +507,21 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5609</v>
+        <v>7192</v>
       </c>
       <c r="D4" t="n">
-        <v>453</v>
+        <v>266</v>
       </c>
       <c r="E4" t="n">
-        <v>1662</v>
+        <v>505</v>
       </c>
       <c r="F4" t="n">
-        <v>468</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -529,21 +529,21 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4563</v>
+        <v>7164</v>
       </c>
       <c r="D5" t="n">
-        <v>1358</v>
+        <v>434</v>
       </c>
       <c r="E5" t="n">
-        <v>961</v>
+        <v>271</v>
       </c>
       <c r="F5" t="n">
-        <v>1310</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -551,21 +551,21 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5554</v>
+        <v>7216</v>
       </c>
       <c r="D6" t="n">
-        <v>491</v>
+        <v>253</v>
       </c>
       <c r="E6" t="n">
-        <v>1650</v>
+        <v>490</v>
       </c>
       <c r="F6" t="n">
-        <v>497</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -573,21 +573,21 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4621</v>
+        <v>7180</v>
       </c>
       <c r="D7" t="n">
-        <v>1400</v>
+        <v>350</v>
       </c>
       <c r="E7" t="n">
-        <v>845</v>
+        <v>306</v>
       </c>
       <c r="F7" t="n">
-        <v>1326</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -595,21 +595,21 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5604</v>
+        <v>7187</v>
       </c>
       <c r="D8" t="n">
-        <v>477</v>
+        <v>256</v>
       </c>
       <c r="E8" t="n">
-        <v>1649</v>
+        <v>509</v>
       </c>
       <c r="F8" t="n">
-        <v>462</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -617,21 +617,21 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4605</v>
+        <v>7181</v>
       </c>
       <c r="D9" t="n">
-        <v>1412</v>
+        <v>393</v>
       </c>
       <c r="E9" t="n">
-        <v>853</v>
+        <v>311</v>
       </c>
       <c r="F9" t="n">
-        <v>1322</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -639,21 +639,21 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>5595</v>
+        <v>7245</v>
       </c>
       <c r="D10" t="n">
-        <v>484</v>
+        <v>242</v>
       </c>
       <c r="E10" t="n">
-        <v>1621</v>
+        <v>483</v>
       </c>
       <c r="F10" t="n">
-        <v>492</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -661,21 +661,21 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4522</v>
+        <v>7105</v>
       </c>
       <c r="D11" t="n">
-        <v>1434</v>
+        <v>418</v>
       </c>
       <c r="E11" t="n">
-        <v>910</v>
+        <v>327</v>
       </c>
       <c r="F11" t="n">
-        <v>1326</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -683,21 +683,21 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5554</v>
+        <v>7218</v>
       </c>
       <c r="D12" t="n">
-        <v>506</v>
+        <v>253</v>
       </c>
       <c r="E12" t="n">
-        <v>1653</v>
+        <v>496</v>
       </c>
       <c r="F12" t="n">
-        <v>479</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -705,21 +705,21 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4632</v>
+        <v>7093</v>
       </c>
       <c r="D13" t="n">
-        <v>1373</v>
+        <v>430</v>
       </c>
       <c r="E13" t="n">
-        <v>878</v>
+        <v>322</v>
       </c>
       <c r="F13" t="n">
-        <v>1309</v>
+        <v>347</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -727,21 +727,21 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5630</v>
+        <v>7206</v>
       </c>
       <c r="D14" t="n">
-        <v>466</v>
+        <v>252</v>
       </c>
       <c r="E14" t="n">
-        <v>1621</v>
+        <v>469</v>
       </c>
       <c r="F14" t="n">
-        <v>475</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -749,21 +749,21 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4589</v>
+        <v>7126</v>
       </c>
       <c r="D15" t="n">
-        <v>1400</v>
+        <v>380</v>
       </c>
       <c r="E15" t="n">
-        <v>925</v>
+        <v>310</v>
       </c>
       <c r="F15" t="n">
-        <v>1278</v>
+        <v>376</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -771,21 +771,21 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5615</v>
+        <v>7234</v>
       </c>
       <c r="D16" t="n">
-        <v>450</v>
+        <v>255</v>
       </c>
       <c r="E16" t="n">
-        <v>1641</v>
+        <v>467</v>
       </c>
       <c r="F16" t="n">
-        <v>486</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -793,21 +793,21 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4459</v>
+        <v>7154</v>
       </c>
       <c r="D17" t="n">
-        <v>1432</v>
+        <v>402</v>
       </c>
       <c r="E17" t="n">
-        <v>937</v>
+        <v>305</v>
       </c>
       <c r="F17" t="n">
-        <v>1364</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -815,21 +815,21 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5601</v>
+        <v>7224</v>
       </c>
       <c r="D18" t="n">
-        <v>485</v>
+        <v>254</v>
       </c>
       <c r="E18" t="n">
-        <v>1613</v>
+        <v>503</v>
       </c>
       <c r="F18" t="n">
-        <v>493</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -837,21 +837,21 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4664</v>
+        <v>7129</v>
       </c>
       <c r="D19" t="n">
-        <v>1342</v>
+        <v>396</v>
       </c>
       <c r="E19" t="n">
-        <v>881</v>
+        <v>331</v>
       </c>
       <c r="F19" t="n">
-        <v>1305</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -859,21 +859,21 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5554</v>
+        <v>7150</v>
       </c>
       <c r="D20" t="n">
-        <v>500</v>
+        <v>255</v>
       </c>
       <c r="E20" t="n">
-        <v>1664</v>
+        <v>513</v>
       </c>
       <c r="F20" t="n">
-        <v>474</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -881,21 +881,21 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>4619</v>
+        <v>7099</v>
       </c>
       <c r="D21" t="n">
-        <v>1349</v>
+        <v>422</v>
       </c>
       <c r="E21" t="n">
-        <v>932</v>
+        <v>334</v>
       </c>
       <c r="F21" t="n">
-        <v>1292</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -903,21 +903,21 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5530</v>
+        <v>7233</v>
       </c>
       <c r="D22" t="n">
-        <v>489</v>
+        <v>254</v>
       </c>
       <c r="E22" t="n">
-        <v>1706</v>
+        <v>473</v>
       </c>
       <c r="F22" t="n">
-        <v>467</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -925,21 +925,21 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4604</v>
+        <v>7130</v>
       </c>
       <c r="D23" t="n">
-        <v>1367</v>
+        <v>400</v>
       </c>
       <c r="E23" t="n">
-        <v>924</v>
+        <v>320</v>
       </c>
       <c r="F23" t="n">
-        <v>1297</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -947,21 +947,21 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>5583</v>
+        <v>7176</v>
       </c>
       <c r="D24" t="n">
-        <v>466</v>
+        <v>248</v>
       </c>
       <c r="E24" t="n">
-        <v>1660</v>
+        <v>520</v>
       </c>
       <c r="F24" t="n">
-        <v>483</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -969,21 +969,21 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4668</v>
+        <v>7179</v>
       </c>
       <c r="D25" t="n">
-        <v>1359</v>
+        <v>388</v>
       </c>
       <c r="E25" t="n">
-        <v>833</v>
+        <v>291</v>
       </c>
       <c r="F25" t="n">
-        <v>1332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -991,21 +991,21 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5597</v>
+        <v>7194</v>
       </c>
       <c r="D26" t="n">
-        <v>486</v>
+        <v>268</v>
       </c>
       <c r="E26" t="n">
-        <v>1627</v>
+        <v>481</v>
       </c>
       <c r="F26" t="n">
-        <v>482</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1013,21 +1013,21 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4604</v>
+        <v>7165</v>
       </c>
       <c r="D27" t="n">
-        <v>1367</v>
+        <v>422</v>
       </c>
       <c r="E27" t="n">
-        <v>869</v>
+        <v>308</v>
       </c>
       <c r="F27" t="n">
-        <v>1352</v>
+        <v>297</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1035,21 +1035,21 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>5641</v>
+        <v>7190</v>
       </c>
       <c r="D28" t="n">
-        <v>500</v>
+        <v>292</v>
       </c>
       <c r="E28" t="n">
-        <v>1606</v>
+        <v>462</v>
       </c>
       <c r="F28" t="n">
-        <v>445</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1057,21 +1057,21 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>4557</v>
+        <v>7118</v>
       </c>
       <c r="D29" t="n">
-        <v>1363</v>
+        <v>415</v>
       </c>
       <c r="E29" t="n">
-        <v>929</v>
+        <v>299</v>
       </c>
       <c r="F29" t="n">
-        <v>1343</v>
+        <v>360</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1079,21 +1079,21 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>5518</v>
+        <v>7218</v>
       </c>
       <c r="D30" t="n">
-        <v>502</v>
+        <v>245</v>
       </c>
       <c r="E30" t="n">
-        <v>1699</v>
+        <v>504</v>
       </c>
       <c r="F30" t="n">
-        <v>473</v>
+        <v>225</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1101,21 +1101,21 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>4521</v>
+        <v>7176</v>
       </c>
       <c r="D31" t="n">
-        <v>1464</v>
+        <v>364</v>
       </c>
       <c r="E31" t="n">
-        <v>890</v>
+        <v>326</v>
       </c>
       <c r="F31" t="n">
-        <v>1317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1123,21 +1123,21 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5588</v>
+        <v>7151</v>
       </c>
       <c r="D32" t="n">
-        <v>514</v>
+        <v>277</v>
       </c>
       <c r="E32" t="n">
-        <v>1613</v>
+        <v>517</v>
       </c>
       <c r="F32" t="n">
-        <v>477</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1145,21 +1145,21 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>4577</v>
+        <v>7185</v>
       </c>
       <c r="D33" t="n">
-        <v>1408</v>
+        <v>386</v>
       </c>
       <c r="E33" t="n">
-        <v>886</v>
+        <v>299</v>
       </c>
       <c r="F33" t="n">
-        <v>1321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1167,21 +1167,21 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>5575</v>
+        <v>7228</v>
       </c>
       <c r="D34" t="n">
-        <v>497</v>
+        <v>255</v>
       </c>
       <c r="E34" t="n">
-        <v>1625</v>
+        <v>479</v>
       </c>
       <c r="F34" t="n">
-        <v>495</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1189,21 +1189,21 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>4566</v>
+        <v>7096</v>
       </c>
       <c r="D35" t="n">
-        <v>1388</v>
+        <v>441</v>
       </c>
       <c r="E35" t="n">
-        <v>923</v>
+        <v>322</v>
       </c>
       <c r="F35" t="n">
-        <v>1315</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1211,21 +1211,21 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5516</v>
+        <v>7189</v>
       </c>
       <c r="D36" t="n">
-        <v>473</v>
+        <v>263</v>
       </c>
       <c r="E36" t="n">
-        <v>1730</v>
+        <v>516</v>
       </c>
       <c r="F36" t="n">
-        <v>473</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1233,21 +1233,21 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>4536</v>
+        <v>7232</v>
       </c>
       <c r="D37" t="n">
-        <v>1375</v>
+        <v>364</v>
       </c>
       <c r="E37" t="n">
-        <v>948</v>
+        <v>287</v>
       </c>
       <c r="F37" t="n">
-        <v>1333</v>
+        <v>309</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1255,21 +1255,21 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>5631</v>
+        <v>7251</v>
       </c>
       <c r="D38" t="n">
-        <v>502</v>
+        <v>241</v>
       </c>
       <c r="E38" t="n">
-        <v>1621</v>
+        <v>463</v>
       </c>
       <c r="F38" t="n">
-        <v>438</v>
+        <v>237</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1277,21 +1277,21 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4634</v>
+        <v>7174</v>
       </c>
       <c r="D39" t="n">
-        <v>1369</v>
+        <v>387</v>
       </c>
       <c r="E39" t="n">
-        <v>920</v>
+        <v>289</v>
       </c>
       <c r="F39" t="n">
-        <v>1269</v>
+        <v>342</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1299,21 +1299,21 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>5586</v>
+        <v>7269</v>
       </c>
       <c r="D40" t="n">
-        <v>512</v>
+        <v>238</v>
       </c>
       <c r="E40" t="n">
-        <v>1660</v>
+        <v>451</v>
       </c>
       <c r="F40" t="n">
-        <v>434</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1321,21 +1321,21 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>4632</v>
+        <v>7119</v>
       </c>
       <c r="D41" t="n">
-        <v>1312</v>
+        <v>397</v>
       </c>
       <c r="E41" t="n">
-        <v>919</v>
+        <v>321</v>
       </c>
       <c r="F41" t="n">
-        <v>1329</v>
+        <v>355</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1343,21 +1343,21 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>5541</v>
+        <v>7207</v>
       </c>
       <c r="D42" t="n">
-        <v>509</v>
+        <v>267</v>
       </c>
       <c r="E42" t="n">
-        <v>1643</v>
+        <v>481</v>
       </c>
       <c r="F42" t="n">
-        <v>499</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1365,21 +1365,21 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>4637</v>
+        <v>7155</v>
       </c>
       <c r="D43" t="n">
-        <v>1401</v>
+        <v>389</v>
       </c>
       <c r="E43" t="n">
-        <v>889</v>
+        <v>305</v>
       </c>
       <c r="F43" t="n">
-        <v>1265</v>
+        <v>343</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1387,21 +1387,21 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>5558</v>
+        <v>7149</v>
       </c>
       <c r="D44" t="n">
-        <v>482</v>
+        <v>269</v>
       </c>
       <c r="E44" t="n">
-        <v>1661</v>
+        <v>536</v>
       </c>
       <c r="F44" t="n">
-        <v>491</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1409,21 +1409,21 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4579</v>
+        <v>7114</v>
       </c>
       <c r="D45" t="n">
-        <v>1402</v>
+        <v>396</v>
       </c>
       <c r="E45" t="n">
-        <v>915</v>
+        <v>320</v>
       </c>
       <c r="F45" t="n">
-        <v>1296</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1431,21 +1431,21 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>5591</v>
+        <v>7196</v>
       </c>
       <c r="D46" t="n">
-        <v>476</v>
+        <v>260</v>
       </c>
       <c r="E46" t="n">
-        <v>1633</v>
+        <v>512</v>
       </c>
       <c r="F46" t="n">
-        <v>492</v>
+        <v>224</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1453,21 +1453,21 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>4486</v>
+        <v>7079</v>
       </c>
       <c r="D47" t="n">
-        <v>1413</v>
+        <v>422</v>
       </c>
       <c r="E47" t="n">
-        <v>929</v>
+        <v>334</v>
       </c>
       <c r="F47" t="n">
-        <v>1364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1475,21 +1475,21 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>5567</v>
+        <v>7193</v>
       </c>
       <c r="D48" t="n">
-        <v>456</v>
+        <v>275</v>
       </c>
       <c r="E48" t="n">
-        <v>1699</v>
+        <v>503</v>
       </c>
       <c r="F48" t="n">
-        <v>470</v>
+        <v>221</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1497,21 +1497,21 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4639</v>
+        <v>7142</v>
       </c>
       <c r="D49" t="n">
-        <v>1395</v>
+        <v>405</v>
       </c>
       <c r="E49" t="n">
-        <v>870</v>
+        <v>305</v>
       </c>
       <c r="F49" t="n">
-        <v>1288</v>
+        <v>340</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1519,21 +1519,21 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>5522</v>
+        <v>7185</v>
       </c>
       <c r="D50" t="n">
-        <v>488</v>
+        <v>252</v>
       </c>
       <c r="E50" t="n">
-        <v>1693</v>
+        <v>481</v>
       </c>
       <c r="F50" t="n">
-        <v>489</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -1541,21 +1541,21 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4552</v>
+        <v>7180</v>
       </c>
       <c r="D51" t="n">
-        <v>1432</v>
+        <v>384</v>
       </c>
       <c r="E51" t="n">
-        <v>916</v>
+        <v>301</v>
       </c>
       <c r="F51" t="n">
-        <v>1292</v>
+        <v>327</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1563,21 +1563,21 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>5678</v>
+        <v>7188</v>
       </c>
       <c r="D52" t="n">
-        <v>478</v>
+        <v>265</v>
       </c>
       <c r="E52" t="n">
-        <v>1588</v>
+        <v>475</v>
       </c>
       <c r="F52" t="n">
-        <v>448</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1585,21 +1585,21 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>4552</v>
+        <v>7191</v>
       </c>
       <c r="D53" t="n">
-        <v>1431</v>
+        <v>387</v>
       </c>
       <c r="E53" t="n">
-        <v>932</v>
+        <v>289</v>
       </c>
       <c r="F53" t="n">
-        <v>1277</v>
+        <v>325</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -1607,21 +1607,21 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>5544</v>
+        <v>7107</v>
       </c>
       <c r="D54" t="n">
-        <v>476</v>
+        <v>294</v>
       </c>
       <c r="E54" t="n">
-        <v>1637</v>
+        <v>542</v>
       </c>
       <c r="F54" t="n">
-        <v>535</v>
+        <v>249</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -1629,21 +1629,21 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>4585</v>
+        <v>7097</v>
       </c>
       <c r="D55" t="n">
-        <v>1369</v>
+        <v>426</v>
       </c>
       <c r="E55" t="n">
-        <v>906</v>
+        <v>303</v>
       </c>
       <c r="F55" t="n">
-        <v>1332</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -1651,21 +1651,21 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5518</v>
+        <v>7148</v>
       </c>
       <c r="D56" t="n">
-        <v>521</v>
+        <v>249</v>
       </c>
       <c r="E56" t="n">
-        <v>1667</v>
+        <v>532</v>
       </c>
       <c r="F56" t="n">
-        <v>486</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -1673,21 +1673,21 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>4620</v>
+        <v>7135</v>
       </c>
       <c r="D57" t="n">
-        <v>1398</v>
+        <v>412</v>
       </c>
       <c r="E57" t="n">
-        <v>897</v>
+        <v>301</v>
       </c>
       <c r="F57" t="n">
-        <v>1277</v>
+        <v>344</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -1695,21 +1695,21 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>5607</v>
+        <v>7153</v>
       </c>
       <c r="D58" t="n">
-        <v>506</v>
+        <v>260</v>
       </c>
       <c r="E58" t="n">
-        <v>1618</v>
+        <v>516</v>
       </c>
       <c r="F58" t="n">
-        <v>461</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -1717,21 +1717,21 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>4632</v>
+        <v>7081</v>
       </c>
       <c r="D59" t="n">
-        <v>1348</v>
+        <v>409</v>
       </c>
       <c r="E59" t="n">
-        <v>907</v>
+        <v>344</v>
       </c>
       <c r="F59" t="n">
-        <v>1305</v>
+        <v>358</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -1739,21 +1739,21 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>5585</v>
+        <v>7233</v>
       </c>
       <c r="D60" t="n">
-        <v>483</v>
+        <v>252</v>
       </c>
       <c r="E60" t="n">
-        <v>1636</v>
+        <v>475</v>
       </c>
       <c r="F60" t="n">
-        <v>488</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -1761,21 +1761,21 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>4623</v>
+        <v>7134</v>
       </c>
       <c r="D61" t="n">
-        <v>1381</v>
+        <v>432</v>
       </c>
       <c r="E61" t="n">
-        <v>885</v>
+        <v>285</v>
       </c>
       <c r="F61" t="n">
-        <v>1303</v>
+        <v>341</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -1783,21 +1783,21 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>5577</v>
+        <v>7168</v>
       </c>
       <c r="D62" t="n">
-        <v>486</v>
+        <v>265</v>
       </c>
       <c r="E62" t="n">
-        <v>1646</v>
+        <v>505</v>
       </c>
       <c r="F62" t="n">
-        <v>483</v>
+        <v>254</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -1805,21 +1805,21 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>4593</v>
+        <v>7167</v>
       </c>
       <c r="D63" t="n">
-        <v>1396</v>
+        <v>382</v>
       </c>
       <c r="E63" t="n">
-        <v>867</v>
+        <v>303</v>
       </c>
       <c r="F63" t="n">
-        <v>1336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -1827,21 +1827,21 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>5640</v>
+        <v>7233</v>
       </c>
       <c r="D64" t="n">
-        <v>466</v>
+        <v>241</v>
       </c>
       <c r="E64" t="n">
-        <v>1644</v>
+        <v>486</v>
       </c>
       <c r="F64" t="n">
-        <v>442</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -1849,21 +1849,21 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>4583</v>
+        <v>7161</v>
       </c>
       <c r="D65" t="n">
-        <v>1370</v>
+        <v>391</v>
       </c>
       <c r="E65" t="n">
-        <v>865</v>
+        <v>327</v>
       </c>
       <c r="F65" t="n">
-        <v>1374</v>
+        <v>313</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -1871,21 +1871,21 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>5634</v>
+        <v>7234</v>
       </c>
       <c r="D66" t="n">
-        <v>497</v>
+        <v>245</v>
       </c>
       <c r="E66" t="n">
-        <v>1593</v>
+        <v>476</v>
       </c>
       <c r="F66" t="n">
-        <v>468</v>
+        <v>237</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -1893,21 +1893,21 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>4572</v>
+        <v>7158</v>
       </c>
       <c r="D67" t="n">
-        <v>1379</v>
+        <v>411</v>
       </c>
       <c r="E67" t="n">
-        <v>937</v>
+        <v>305</v>
       </c>
       <c r="F67" t="n">
-        <v>1304</v>
+        <v>318</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -1915,21 +1915,21 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>5623</v>
+        <v>7179</v>
       </c>
       <c r="D68" t="n">
-        <v>468</v>
+        <v>268</v>
       </c>
       <c r="E68" t="n">
-        <v>1603</v>
+        <v>513</v>
       </c>
       <c r="F68" t="n">
-        <v>498</v>
+        <v>232</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -1937,21 +1937,21 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>4522</v>
+        <v>7155</v>
       </c>
       <c r="D69" t="n">
-        <v>1427</v>
+        <v>401</v>
       </c>
       <c r="E69" t="n">
-        <v>948</v>
+        <v>289</v>
       </c>
       <c r="F69" t="n">
-        <v>1295</v>
+        <v>347</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -1959,21 +1959,21 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>5617</v>
+        <v>7200</v>
       </c>
       <c r="D70" t="n">
-        <v>481</v>
+        <v>255</v>
       </c>
       <c r="E70" t="n">
-        <v>1599</v>
+        <v>509</v>
       </c>
       <c r="F70" t="n">
-        <v>495</v>
+        <v>228</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -1981,21 +1981,21 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>4607</v>
+        <v>7175</v>
       </c>
       <c r="D71" t="n">
-        <v>1347</v>
+        <v>391</v>
       </c>
       <c r="E71" t="n">
-        <v>915</v>
+        <v>305</v>
       </c>
       <c r="F71" t="n">
-        <v>1323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -2003,21 +2003,21 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>5576</v>
+        <v>7204</v>
       </c>
       <c r="D72" t="n">
-        <v>464</v>
+        <v>241</v>
       </c>
       <c r="E72" t="n">
-        <v>1646</v>
+        <v>501</v>
       </c>
       <c r="F72" t="n">
-        <v>506</v>
+        <v>246</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -2025,21 +2025,21 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>4499</v>
+        <v>7152</v>
       </c>
       <c r="D73" t="n">
-        <v>1362</v>
+        <v>390</v>
       </c>
       <c r="E73" t="n">
-        <v>953</v>
+        <v>317</v>
       </c>
       <c r="F73" t="n">
-        <v>1378</v>
+        <v>333</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2047,21 +2047,21 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>5625</v>
+        <v>7154</v>
       </c>
       <c r="D74" t="n">
-        <v>482</v>
+        <v>286</v>
       </c>
       <c r="E74" t="n">
-        <v>1630</v>
+        <v>499</v>
       </c>
       <c r="F74" t="n">
-        <v>455</v>
+        <v>253</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1619752193.191894</v>
+        <v>1621310783.646369</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -2069,16 +2069,16 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>4630</v>
+        <v>7137</v>
       </c>
       <c r="D75" t="n">
-        <v>1368</v>
+        <v>429</v>
       </c>
       <c r="E75" t="n">
-        <v>864</v>
+        <v>291</v>
       </c>
       <c r="F75" t="n">
-        <v>1330</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>